<commit_message>
Update tRNAscan procedure to include legacy search, updated tRNAs
</commit_message>
<xml_diff>
--- a/Bacilli_AGG_Met/Bacilli_AGG_Met_genomes_info.xlsx
+++ b/Bacilli_AGG_Met/Bacilli_AGG_Met_genomes_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shulgina/Google Drive/genetic code paper/new_genetic_code_evidence/Bacilli_AGG_Met/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shulgina/Google Drive/genetic code paper/ShulginaEddy_21_genetic_codes/Bacilli_AGG_Met/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EB0FE1-CCAD-2946-A32C-A2C249D81FA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB90F717-F793-7845-9F55-BCF443BAA3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="48960" windowHeight="31540" xr2:uid="{43D3B795-32D0-1D4C-A93F-C3CF537C0D08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{43D3B795-32D0-1D4C-A93F-C3CF537C0D08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A9A72D-EA13-8843-AE70-1604CB32D78C}">
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>1.12E-2</v>
       </c>
       <c r="L13" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="10">
         <v>0</v>
@@ -1783,19 +1783,19 @@
         <v>0</v>
       </c>
       <c r="O13" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13" s="4">
         <v>6.1</v>
@@ -2096,28 +2096,28 @@
         <v>0</v>
       </c>
       <c r="L17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="10">
         <v>0</v>
       </c>
       <c r="N17" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="4">
         <v>37</v>

</xml_diff>